<commit_message>
Finished writing and QA the generate function, added new gui to the project.
</commit_message>
<xml_diff>
--- a/ilutzim.xlsx
+++ b/ilutzim.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Python\Automatic schedule generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA37073F-5F6A-4A73-A0E7-B384979D19F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE32E55-745B-43F1-BAC1-1B4FA0378CAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Manager" sheetId="1" r:id="rId1"/>
-    <sheet name="Makel Officer" sheetId="2" r:id="rId2"/>
+    <sheet name="Makel Officer" sheetId="1" r:id="rId1"/>
+    <sheet name="Manager" sheetId="2" r:id="rId2"/>
     <sheet name="Makel Operator" sheetId="3" r:id="rId3"/>
     <sheet name="Samba" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -23,59 +23,62 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="28">
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3+4</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
     <t>יועד בוגנר</t>
   </si>
   <si>
+    <t>אפק בן סימון</t>
+  </si>
+  <si>
     <t>שלי מועלם</t>
   </si>
   <si>
-    <t>אפק בן סימון</t>
+    <t>הודיה צפדיה</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>תומר שניידר</t>
   </si>
   <si>
     <t>עמית גריסרו</t>
   </si>
   <si>
-    <t>תומר שניידר</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Team</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3+4</t>
-  </si>
-  <si>
     <t>יובל אבידן</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>יואב שוומנטל</t>
   </si>
   <si>
@@ -85,10 +88,13 @@
     <t>רוני שור</t>
   </si>
   <si>
-    <t>דב סולומון</t>
-  </si>
-  <si>
-    <t>סיון שליו</t>
+    <t>עדו בורנשטיין</t>
+  </si>
+  <si>
+    <t>תומר ארליכמן</t>
+  </si>
+  <si>
+    <t>לוטן תמרי</t>
   </si>
   <si>
     <t>רוני בורט</t>
@@ -100,34 +106,20 @@
     <t>אמבר פרץ</t>
   </si>
   <si>
-    <t>שקד יעקב</t>
-  </si>
-  <si>
-    <t>לוטן תמרי</t>
-  </si>
-  <si>
-    <t>עדו בורנשטיין</t>
-  </si>
-  <si>
-    <t>נטע לאופר</t>
+    <t>רומי שוחט</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -143,51 +135,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -233,24 +186,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,136 +498,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -691,78 +506,78 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="3" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="5"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -803,7 +618,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -844,7 +659,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -885,43 +700,43 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -935,100 +750,303 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="6" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="8"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>14</v>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
+      <c r="A5" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1068,8 +1086,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
+      <c r="A6" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1109,126 +1127,44 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1244,37 +1180,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1286,35 +1222,35 @@
         <v>0</v>
       </c>
       <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1326,15 +1262,15 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1350,7 +1286,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -1366,15 +1302,15 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1390,11 +1326,11 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1410,11 +1346,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1430,83 +1366,43 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>